<commit_message>
fix small bug, where it would crash in a weird way if the incorrect column name was given
</commit_message>
<xml_diff>
--- a/data/shapefilekarteringinfo.xlsx
+++ b/data/shapefilekarteringinfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jordydelange\git\veg2hab\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mark\git\veg2hab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDDA7FD-F20C-488F-A6E9-98A4475EF0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB0BC7C-FDF6-4BEE-AA7E-AAF94B1DE421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21150" xr2:uid="{A4E3BD7C-813B-4E93-85DC-065BC75D0463}"/>
+    <workbookView xWindow="28680" yWindow="-3510" windowWidth="51840" windowHeight="21240" xr2:uid="{A4E3BD7C-813B-4E93-85DC-065BC75D0463}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -857,7 +857,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,7 +1218,7 @@
         <v>64</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>122</v>

</xml_diff>